<commit_message>
"p -10, inicio acel 10"
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -490,13 +490,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10.40552080389987</v>
+        <v>10.41083696637312</v>
       </c>
       <c r="E2" t="n">
-        <v>88</v>
+        <v>10000</v>
       </c>
       <c r="F2" t="n">
-        <v>9.438021135481325e-06</v>
+        <v>9.025885347604574e-10</v>
       </c>
       <c r="G2" t="n">
         <v>398</v>
@@ -527,13 +527,13 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10.26974106120281</v>
+        <v>10.41064597649401</v>
       </c>
       <c r="E3" t="n">
-        <v>31</v>
+        <v>6652</v>
       </c>
       <c r="F3" t="n">
-        <v>6.252801378209473e-06</v>
+        <v>7.061195356961412e-11</v>
       </c>
       <c r="G3" t="n">
         <v>398</v>
@@ -564,13 +564,13 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>10.40353710214386</v>
+        <v>10.40660457794342</v>
       </c>
       <c r="E4" t="n">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="F4" t="n">
-        <v>9.342798923266315e-06</v>
+        <v>6.732421208540055e-11</v>
       </c>
       <c r="G4" t="n">
         <v>398</v>
@@ -601,13 +601,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>10.40295727705686</v>
+        <v>10.40660333716813</v>
       </c>
       <c r="E5" t="n">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="F5" t="n">
-        <v>9.218623557247631e-06</v>
+        <v>6.938399862840957e-11</v>
       </c>
       <c r="G5" t="n">
         <v>398</v>
@@ -712,13 +712,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10.40353710214386</v>
+        <v>10.40660457794342</v>
       </c>
       <c r="E8" t="n">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="F8" t="n">
-        <v>9.346855024441101e-06</v>
+        <v>6.782656788632418e-11</v>
       </c>
       <c r="G8" t="n">
         <v>398</v>
@@ -749,13 +749,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10.34603941058515</v>
+        <v>10.40660291773662</v>
       </c>
       <c r="E9" t="n">
-        <v>41</v>
+        <v>174</v>
       </c>
       <c r="F9" t="n">
-        <v>9.954929419974046e-06</v>
+        <v>7.387721035772134e-11</v>
       </c>
       <c r="G9" t="n">
         <v>398</v>
@@ -786,13 +786,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>199.9997138985918</v>
+        <v>199.9999999956344</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F10" t="n">
-        <v>4.291474057006672e-06</v>
+        <v>6.548376063762736e-11</v>
       </c>
       <c r="G10" t="n">
         <v>48</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>199.9816930845243</v>
+        <v>199.9999284744817</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F11" t="n">
-        <v>4.353826715540065e-06</v>
+        <v>6.650680006685051e-11</v>
       </c>
       <c r="G11" t="n">
         <v>48</v>
@@ -860,13 +860,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>199.9999955296518</v>
+        <v>199.9999999999829</v>
       </c>
       <c r="E12" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F12" t="n">
-        <v>9.212843238718603e-06</v>
+        <v>3.517286017872089e-11</v>
       </c>
       <c r="G12" t="n">
         <v>48</v>
@@ -897,13 +897,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>199.9999955296518</v>
+        <v>199.9999999999829</v>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F13" t="n">
-        <v>8.120659239250246e-06</v>
+        <v>3.283560090387037e-11</v>
       </c>
       <c r="G13" t="n">
         <v>48</v>
@@ -1008,13 +1008,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>199.9999955296518</v>
+        <v>199.9999999999829</v>
       </c>
       <c r="E16" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F16" t="n">
-        <v>9.21299168555926e-06</v>
+        <v>3.502933054610741e-11</v>
       </c>
       <c r="G16" t="n">
         <v>48</v>
@@ -1045,13 +1045,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>199.9999955296518</v>
+        <v>199.9999999999829</v>
       </c>
       <c r="E17" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F17" t="n">
-        <v>9.293305930451898e-06</v>
+        <v>3.550752580976184e-11</v>
       </c>
       <c r="G17" t="n">
         <v>48</v>
@@ -1082,13 +1082,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>6197043.861659037</v>
+        <v>6197287.051397814</v>
       </c>
       <c r="E18" t="n">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="F18" t="n">
-        <v>8.936504241502064e-06</v>
+        <v>9.691242166203807e-11</v>
       </c>
       <c r="G18" t="n">
         <v>153</v>
@@ -1119,13 +1119,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>6193373.021736953</v>
+        <v>6197285.757615398</v>
       </c>
       <c r="E19" t="n">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="F19" t="n">
-        <v>9.506735145473922e-06</v>
+        <v>9.54792100668907e-11</v>
       </c>
       <c r="G19" t="n">
         <v>153</v>
@@ -1156,13 +1156,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>6197121.325827673</v>
+        <v>6197287.048449507</v>
       </c>
       <c r="E20" t="n">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="F20" t="n">
-        <v>7.558275077303443e-06</v>
+        <v>9.402571091828995e-11</v>
       </c>
       <c r="G20" t="n">
         <v>153</v>
@@ -1193,13 +1193,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>6197087.151238746</v>
+        <v>6197287.047441144</v>
       </c>
       <c r="E21" t="n">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="F21" t="n">
-        <v>8.936521690750358e-06</v>
+        <v>6.832363075419507e-11</v>
       </c>
       <c r="G21" t="n">
         <v>153</v>
@@ -1304,13 +1304,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6197121.325827673</v>
+        <v>6197287.048449507</v>
       </c>
       <c r="E24" t="n">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="F24" t="n">
-        <v>7.558722902285141e-06</v>
+        <v>9.378466327958547e-11</v>
       </c>
       <c r="G24" t="n">
         <v>153</v>
@@ -1341,13 +1341,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>6196823.717917441</v>
+        <v>6197286.989795357</v>
       </c>
       <c r="E25" t="n">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="F25" t="n">
-        <v>8.929744223888457e-06</v>
+        <v>8.360761474517046e-11</v>
       </c>
       <c r="G25" t="n">
         <v>153</v>
@@ -1378,13 +1378,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>30115.82629984464</v>
+        <v>30148.79411856191</v>
       </c>
       <c r="E26" t="n">
-        <v>22</v>
+        <v>1231</v>
       </c>
       <c r="F26" t="n">
-        <v>9.397377028680276e-06</v>
+        <v>9.906775418343501e-11</v>
       </c>
       <c r="G26" t="n">
         <v>1138</v>
@@ -1415,13 +1415,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>30101.60734657212</v>
+        <v>30148.6402523005</v>
       </c>
       <c r="E27" t="n">
-        <v>14</v>
+        <v>595</v>
       </c>
       <c r="F27" t="n">
-        <v>4.186377565356223e-06</v>
+        <v>9.654664719054071e-11</v>
       </c>
       <c r="G27" t="n">
         <v>1138</v>
@@ -1452,13 +1452,13 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>30116.09139544879</v>
+        <v>30148.78281109525</v>
       </c>
       <c r="E28" t="n">
-        <v>23</v>
+        <v>859</v>
       </c>
       <c r="F28" t="n">
-        <v>6.485448959809388e-06</v>
+        <v>9.609852570279945e-11</v>
       </c>
       <c r="G28" t="n">
         <v>1138</v>
@@ -1489,13 +1489,13 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>30116.09139544879</v>
+        <v>30135.17405261119</v>
       </c>
       <c r="E29" t="n">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="F29" t="n">
-        <v>4.535381758166918e-06</v>
+        <v>9.695341624095958e-11</v>
       </c>
       <c r="G29" t="n">
         <v>1138</v>
@@ -1600,13 +1600,13 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>30116.09139544879</v>
+        <v>30148.75084112083</v>
       </c>
       <c r="E32" t="n">
-        <v>23</v>
+        <v>724</v>
       </c>
       <c r="F32" t="n">
-        <v>6.486092513709352e-06</v>
+        <v>6.670350626795326e-11</v>
       </c>
       <c r="G32" t="n">
         <v>1138</v>
@@ -1637,13 +1637,13 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>30115.82629984464</v>
+        <v>30146.64990782431</v>
       </c>
       <c r="E33" t="n">
-        <v>22</v>
+        <v>325</v>
       </c>
       <c r="F33" t="n">
-        <v>8.438909571862254e-06</v>
+        <v>8.378623029590728e-11</v>
       </c>
       <c r="G33" t="n">
         <v>1138</v>
@@ -1674,13 +1674,13 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>5.502385709511155</v>
+        <v>5.502378378978929</v>
       </c>
       <c r="E34" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F34" t="n">
-        <v>3.301034735295559e-06</v>
+        <v>4.614223178292824e-11</v>
       </c>
       <c r="G34" t="n">
         <v>104</v>
@@ -1711,13 +1711,13 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>5.502403873077509</v>
+        <v>5.50237842977301</v>
       </c>
       <c r="E35" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F35" t="n">
-        <v>1.655823763081636e-06</v>
+        <v>6.065363656690676e-11</v>
       </c>
       <c r="G35" t="n">
         <v>104</v>
@@ -1748,13 +1748,13 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>5.502378554904305</v>
+        <v>5.502378378877919</v>
       </c>
       <c r="E36" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F36" t="n">
-        <v>6.398499420325932e-06</v>
+        <v>8.892165939451615e-11</v>
       </c>
       <c r="G36" t="n">
         <v>104</v>
@@ -1785,13 +1785,13 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>5.502378554904305</v>
+        <v>5.502378378877919</v>
       </c>
       <c r="E37" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F37" t="n">
-        <v>5.59858695817911e-06</v>
+        <v>8.274454662063049e-11</v>
       </c>
       <c r="G37" t="n">
         <v>104</v>
@@ -1896,13 +1896,13 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>5.502378554904305</v>
+        <v>5.502378378877919</v>
       </c>
       <c r="E40" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F40" t="n">
-        <v>6.398426297731308e-06</v>
+        <v>8.891972238831549e-11</v>
       </c>
       <c r="G40" t="n">
         <v>104</v>
@@ -1933,13 +1933,13 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>5.502378554904305</v>
+        <v>5.502378378877919</v>
       </c>
       <c r="E41" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F41" t="n">
-        <v>5.996620976232606e-06</v>
+        <v>8.328448708518714e-11</v>
       </c>
       <c r="G41" t="n">
         <v>104</v>
@@ -1970,13 +1970,13 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.9782280548675101</v>
+        <v>0.9788022306513534</v>
       </c>
       <c r="E42" t="n">
-        <v>100</v>
+        <v>4875</v>
       </c>
       <c r="F42" t="n">
-        <v>9.610528240921566e-06</v>
+        <v>9.991530743457809e-11</v>
       </c>
       <c r="G42" t="n">
         <v>2048</v>
@@ -2007,13 +2007,13 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.9769137067289084</v>
+        <v>0.9787919201260611</v>
       </c>
       <c r="E43" t="n">
-        <v>64</v>
+        <v>2234</v>
       </c>
       <c r="F43" t="n">
-        <v>9.407687553626166e-06</v>
+        <v>9.630889006611835e-11</v>
       </c>
       <c r="G43" t="n">
         <v>2048</v>
@@ -2044,13 +2044,13 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.9778200667504259</v>
+        <v>0.9787705852933443</v>
       </c>
       <c r="E44" t="n">
-        <v>79</v>
+        <v>1675</v>
       </c>
       <c r="F44" t="n">
-        <v>9.659187332243112e-06</v>
+        <v>7.899018222984142e-11</v>
       </c>
       <c r="G44" t="n">
         <v>2048</v>
@@ -2081,13 +2081,13 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.9685609508207557</v>
+        <v>0.9785554077148678</v>
       </c>
       <c r="E45" t="n">
-        <v>32</v>
+        <v>545</v>
       </c>
       <c r="F45" t="n">
-        <v>8.446313999518283e-06</v>
+        <v>6.763274964508732e-11</v>
       </c>
       <c r="G45" t="n">
         <v>2048</v>
@@ -2192,13 +2192,13 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.9778200667504259</v>
+        <v>0.9787950509179197</v>
       </c>
       <c r="E48" t="n">
-        <v>79</v>
+        <v>2412</v>
       </c>
       <c r="F48" t="n">
-        <v>9.666406084841957e-06</v>
+        <v>9.53195032114241e-11</v>
       </c>
       <c r="G48" t="n">
         <v>2048</v>
@@ -2229,13 +2229,13 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.9582634984076825</v>
+        <v>0.9784064008082318</v>
       </c>
       <c r="E49" t="n">
-        <v>15</v>
+        <v>205</v>
       </c>
       <c r="F49" t="n">
-        <v>9.111084992032192e-06</v>
+        <v>8.052059947469192e-11</v>
       </c>
       <c r="G49" t="n">
         <v>2048</v>
@@ -2266,13 +2266,13 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>3014181127.26153</v>
+        <v>3015179080.010438</v>
       </c>
       <c r="E50" t="n">
-        <v>134</v>
+        <v>520</v>
       </c>
       <c r="F50" t="n">
-        <v>9.821227875599703e-06</v>
+        <v>9.95572108325373e-11</v>
       </c>
       <c r="G50" t="n">
         <v>48</v>
@@ -2303,13 +2303,13 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>3011156754.072117</v>
+        <v>3015164921.695023</v>
       </c>
       <c r="E51" t="n">
-        <v>85</v>
+        <v>277</v>
       </c>
       <c r="F51" t="n">
-        <v>9.676802385755104e-06</v>
+        <v>9.801165388238914e-11</v>
       </c>
       <c r="G51" t="n">
         <v>48</v>
@@ -2340,13 +2340,13 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2996903287.477822</v>
+        <v>3015178990.986972</v>
       </c>
       <c r="E52" t="n">
-        <v>20</v>
+        <v>443</v>
       </c>
       <c r="F52" t="n">
-        <v>9.879920810874217e-06</v>
+        <v>9.596636076646659e-11</v>
       </c>
       <c r="G52" t="n">
         <v>48</v>
@@ -2377,13 +2377,13 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>2996244213.466879</v>
+        <v>3015178621.431344</v>
       </c>
       <c r="E53" t="n">
-        <v>18</v>
+        <v>391</v>
       </c>
       <c r="F53" t="n">
-        <v>3.027903214592014e-06</v>
+        <v>9.6114871223921e-11</v>
       </c>
       <c r="G53" t="n">
         <v>48</v>
@@ -2488,13 +2488,13 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>2996903287.477822</v>
+        <v>3015178893.111733</v>
       </c>
       <c r="E56" t="n">
-        <v>20</v>
+        <v>420</v>
       </c>
       <c r="F56" t="n">
-        <v>9.927615749139931e-06</v>
+        <v>8.65302926825525e-11</v>
       </c>
       <c r="G56" t="n">
         <v>48</v>
@@ -2525,13 +2525,13 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>2996575918.088687</v>
+        <v>3006240323.348099</v>
       </c>
       <c r="E57" t="n">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="F57" t="n">
-        <v>7.971580623049999e-06</v>
+        <v>1.143794261840101e-11</v>
       </c>
       <c r="G57" t="n">
         <v>48</v>
@@ -2562,13 +2562,13 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>5.502385709075823</v>
+        <v>5.502378378573628</v>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F58" t="n">
-        <v>3.300874632199692e-06</v>
+        <v>4.614239320351041e-11</v>
       </c>
       <c r="G58" t="n">
         <v>400</v>
@@ -2599,13 +2599,13 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>5.502403871761227</v>
+        <v>5.502378429367709</v>
       </c>
       <c r="E59" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F59" t="n">
-        <v>2.432831504630166e-06</v>
+        <v>6.063232950316975e-11</v>
       </c>
       <c r="G59" t="n">
         <v>400</v>
@@ -2636,13 +2636,13 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>5.502378554499002</v>
+        <v>5.502378378472619</v>
       </c>
       <c r="E60" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F60" t="n">
-        <v>6.396470867907771e-06</v>
+        <v>8.88863090379013e-11</v>
       </c>
       <c r="G60" t="n">
         <v>400</v>
@@ -2673,13 +2673,13 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>5.502378554499002</v>
+        <v>5.502378378472619</v>
       </c>
       <c r="E61" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F61" t="n">
-        <v>5.596741800123158e-06</v>
+        <v>8.274131828305741e-11</v>
       </c>
       <c r="G61" t="n">
         <v>400</v>
@@ -2784,13 +2784,13 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>5.502378554499002</v>
+        <v>5.502378378472619</v>
       </c>
       <c r="E64" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F64" t="n">
-        <v>6.396397799388885e-06</v>
+        <v>8.895684834704741e-11</v>
       </c>
       <c r="G64" t="n">
         <v>400</v>
@@ -2821,13 +2821,13 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>5.502378554499002</v>
+        <v>5.502378378472619</v>
       </c>
       <c r="E65" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F65" t="n">
-        <v>5.993704943003528e-06</v>
+        <v>8.249531848194686e-11</v>
       </c>
       <c r="G65" t="n">
         <v>400</v>
@@ -2858,13 +2858,13 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>66.48767021742641</v>
+        <v>66.49656397787049</v>
       </c>
       <c r="E66" t="n">
-        <v>100</v>
+        <v>271</v>
       </c>
       <c r="F66" t="n">
-        <v>9.411786735373271e-06</v>
+        <v>9.581047272545482e-11</v>
       </c>
       <c r="G66" t="n">
         <v>1104</v>
@@ -2895,13 +2895,13 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>65.95354907787359</v>
+        <v>66.49648730538858</v>
       </c>
       <c r="E67" t="n">
-        <v>39</v>
+        <v>170</v>
       </c>
       <c r="F67" t="n">
-        <v>6.35985957088322e-06</v>
+        <v>9.989956374508951e-11</v>
       </c>
       <c r="G67" t="n">
         <v>1104</v>
@@ -2932,13 +2932,13 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>66.46192362411153</v>
+        <v>66.49656370279384</v>
       </c>
       <c r="E68" t="n">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="F68" t="n">
-        <v>9.773860159891637e-06</v>
+        <v>9.681297783983837e-11</v>
       </c>
       <c r="G68" t="n">
         <v>1104</v>
@@ -2969,13 +2969,13 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>66.4540937146667</v>
+        <v>66.49656326260559</v>
       </c>
       <c r="E69" t="n">
-        <v>77</v>
+        <v>238</v>
       </c>
       <c r="F69" t="n">
-        <v>9.530903348866505e-06</v>
+        <v>9.477078382019032e-11</v>
       </c>
       <c r="G69" t="n">
         <v>1104</v>
@@ -3080,13 +3080,13 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>66.46192362411153</v>
+        <v>66.49656367793219</v>
       </c>
       <c r="E72" t="n">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="F72" t="n">
-        <v>9.780754143655196e-06</v>
+        <v>9.422369045765888e-11</v>
       </c>
       <c r="G72" t="n">
         <v>1104</v>
@@ -3117,13 +3117,13 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>65.83631507797743</v>
+        <v>66.49655852666243</v>
       </c>
       <c r="E73" t="n">
-        <v>36</v>
+        <v>209</v>
       </c>
       <c r="F73" t="n">
-        <v>9.62667128097237e-06</v>
+        <v>8.822362850942354e-11</v>
       </c>
       <c r="G73" t="n">
         <v>1104</v>
@@ -3154,13 +3154,13 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>11.86393030934931</v>
+        <v>11.86733830706314</v>
       </c>
       <c r="E74" t="n">
-        <v>113</v>
+        <v>870</v>
       </c>
       <c r="F74" t="n">
-        <v>9.983343197157405e-06</v>
+        <v>9.887665439129894e-11</v>
       </c>
       <c r="G74" t="n">
         <v>900</v>
@@ -3191,13 +3191,13 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>11.79747645891352</v>
+        <v>11.86722648600631</v>
       </c>
       <c r="E75" t="n">
-        <v>49</v>
+        <v>329</v>
       </c>
       <c r="F75" t="n">
-        <v>7.54235882018588e-06</v>
+        <v>9.935833806553928e-11</v>
       </c>
       <c r="G75" t="n">
         <v>900</v>
@@ -3228,13 +3228,13 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>11.85645615888795</v>
+        <v>11.86733623746636</v>
       </c>
       <c r="E76" t="n">
-        <v>85</v>
+        <v>628</v>
       </c>
       <c r="F76" t="n">
-        <v>9.81770735511485e-06</v>
+        <v>7.899347461762838e-11</v>
       </c>
       <c r="G76" t="n">
         <v>900</v>
@@ -3265,13 +3265,13 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>11.85343165531611</v>
+        <v>11.86732786565626</v>
       </c>
       <c r="E77" t="n">
-        <v>80</v>
+        <v>508</v>
       </c>
       <c r="F77" t="n">
-        <v>9.892118321232777e-06</v>
+        <v>3.536210088174771e-11</v>
       </c>
       <c r="G77" t="n">
         <v>900</v>
@@ -3376,13 +3376,13 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>11.85645615888795</v>
+        <v>11.86733586681646</v>
       </c>
       <c r="E80" t="n">
-        <v>85</v>
+        <v>616</v>
       </c>
       <c r="F80" t="n">
-        <v>9.827635608958418e-06</v>
+        <v>7.083267537190448e-11</v>
       </c>
       <c r="G80" t="n">
         <v>900</v>
@@ -3413,13 +3413,13 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>11.73701787012534</v>
+        <v>11.86710093323266</v>
       </c>
       <c r="E81" t="n">
-        <v>37</v>
+        <v>272</v>
       </c>
       <c r="F81" t="n">
-        <v>9.146802698081266e-06</v>
+        <v>7.929097315067625e-11</v>
       </c>
       <c r="G81" t="n">
         <v>900</v>
@@ -3450,13 +3450,13 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>12.41717072759173</v>
+        <v>12.60584912893822</v>
       </c>
       <c r="E82" t="n">
-        <v>233</v>
+        <v>2832</v>
       </c>
       <c r="F82" t="n">
-        <v>1.978124861502015e-06</v>
+        <v>4.536838100943374e-11</v>
       </c>
       <c r="G82" t="n">
         <v>236</v>
@@ -3487,13 +3487,13 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>12.64837768291397</v>
+        <v>12.60584912953977</v>
       </c>
       <c r="E83" t="n">
-        <v>37</v>
+        <v>2833</v>
       </c>
       <c r="F83" t="n">
-        <v>3.152220678864829e-06</v>
+        <v>4.519294147690548e-11</v>
       </c>
       <c r="G83" t="n">
         <v>236</v>
@@ -3524,13 +3524,13 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>12.6570291860012</v>
+        <v>12.60614935431771</v>
       </c>
       <c r="E84" t="n">
-        <v>31</v>
+        <v>1957</v>
       </c>
       <c r="F84" t="n">
-        <v>8.31017484882125e-06</v>
+        <v>1.919079579004e-12</v>
       </c>
       <c r="G84" t="n">
         <v>236</v>
@@ -3561,13 +3561,13 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>12.65532767052682</v>
+        <v>12.60637048546948</v>
       </c>
       <c r="E85" t="n">
-        <v>32</v>
+        <v>1893</v>
       </c>
       <c r="F85" t="n">
-        <v>9.034096133071129e-06</v>
+        <v>4.204879152795875e-11</v>
       </c>
       <c r="G85" t="n">
         <v>236</v>
@@ -3672,13 +3672,13 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>12.6570291860012</v>
+        <v>12.60932751697525</v>
       </c>
       <c r="E88" t="n">
-        <v>31</v>
+        <v>1304</v>
       </c>
       <c r="F88" t="n">
-        <v>8.374639274010006e-06</v>
+        <v>8.831218358091898e-11</v>
       </c>
       <c r="G88" t="n">
         <v>236</v>
@@ -3709,13 +3709,13 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>12.66575276375507</v>
+        <v>12.60185161443958</v>
       </c>
       <c r="E89" t="n">
-        <v>26</v>
+        <v>719</v>
       </c>
       <c r="F89" t="n">
-        <v>7.538010665951079e-06</v>
+        <v>2.779449023045671e-11</v>
       </c>
       <c r="G89" t="n">
         <v>236</v>
@@ -3746,13 +3746,13 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>4359440.548861713</v>
+        <v>4359568.100322182</v>
       </c>
       <c r="E90" t="n">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="F90" t="n">
-        <v>8.017116406457163e-06</v>
+        <v>9.18432711756057e-11</v>
       </c>
       <c r="G90" t="n">
         <v>27</v>
@@ -3783,13 +3783,13 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>4354741.324416467</v>
+        <v>4359559.206934161</v>
       </c>
       <c r="E91" t="n">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="F91" t="n">
-        <v>5.861043871804342e-06</v>
+        <v>9.542921829765347e-11</v>
       </c>
       <c r="G91" t="n">
         <v>27</v>
@@ -3820,13 +3820,13 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>4359467.98054079</v>
+        <v>4359568.100636504</v>
       </c>
       <c r="E92" t="n">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F92" t="n">
-        <v>8.309118035027652e-06</v>
+        <v>9.520576418355374e-11</v>
       </c>
       <c r="G92" t="n">
         <v>27</v>
@@ -3857,13 +3857,13 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>4359440.548861713</v>
+        <v>4359568.100636504</v>
       </c>
       <c r="E93" t="n">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="F93" t="n">
-        <v>9.450585808070602e-06</v>
+        <v>9.028101503111049e-11</v>
       </c>
       <c r="G93" t="n">
         <v>27</v>
@@ -3968,13 +3968,13 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>4359467.98054079</v>
+        <v>4359568.100636504</v>
       </c>
       <c r="E96" t="n">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="F96" t="n">
-        <v>8.309684930382372e-06</v>
+        <v>9.73292191167486e-11</v>
       </c>
       <c r="G96" t="n">
         <v>27</v>
@@ -4005,13 +4005,13 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>4359022.544585026</v>
+        <v>4359568.096880184</v>
       </c>
       <c r="E97" t="n">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F97" t="n">
-        <v>9.034417681731687e-06</v>
+        <v>8.161009838585245e-11</v>
       </c>
       <c r="G97" t="n">
         <v>27</v>

</xml_diff>